<commit_message>
Added -Z end cap connector to 1U
</commit_message>
<xml_diff>
--- a/oresat-backplane-1u-bom.xlsx
+++ b/oresat-backplane-1u-bom.xlsx
@@ -118,7 +118,7 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -175,7 +175,7 @@
     <row r="3" spans="1:18" ht="13.5">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>PCB version: 1.0</t>
+          <t>PCB version: 1.1</t>
         </is>
       </c>
       <c r="B3" s="2"/>
@@ -487,35 +487,82 @@
         </is>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="13.5">
-      <c r="A13" t="inlineStr">
+    <row r="12" spans="1:18" ht="13.5">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>J1</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>5-104196-5</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>20 Position Receptacle Connector  Through Hole, Right Angle</t>
+        </is>
+      </c>
+      <c r="G12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>A115240-ND</t>
+        </is>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="13.5">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Revision versioing infro</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="13.5">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Rev</t>
         </is>
       </c>
     </row>
     <row r="16" spans="1:18" ht="13.5">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Rev</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="13.5">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>1.0r0</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>Initial BOM for 1U.</t>
         </is>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="13.5"/>
-    <row r="1048559" spans="1:18">
-      <c r="I1048559" s="0"/>
+    <row r="18" spans="1:18" ht="13.5">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1.1r0</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Added -Z end cap connector</t>
+        </is>
+      </c>
     </row>
     <row r="1048560" spans="1:18">
       <c r="I1048560" s="0"/>

</xml_diff>

<commit_message>
Added debug connector to 1U BOM.
</commit_message>
<xml_diff>
--- a/oresat-backplane-1u-bom.xlsx
+++ b/oresat-backplane-1u-bom.xlsx
@@ -19,7 +19,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4" count="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="7">
+  <si>
+    <t>Notes</t>
+  </si>
   <si>
     <t>P</t>
   </si>
@@ -32,11 +35,20 @@
   <si>
     <t>Samtec</t>
   </si>
+  <si>
+    <t>Rev</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="100"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <b val="0"/>
@@ -89,7 +101,7 @@
       <protection locked="1" hidden="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
@@ -106,6 +118,10 @@
       <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
       <protection locked="1" hidden="0"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="100" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -118,7 +134,7 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B18" sqref="B18:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -278,10 +294,8 @@
           <t>Generic</t>
         </is>
       </c>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
+      <c r="J6" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="13.5">
@@ -294,7 +308,7 @@
         </is>
       </c>
       <c r="C7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -312,7 +326,7 @@
         </is>
       </c>
       <c r="G7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -320,7 +334,12 @@
         </is>
       </c>
       <c r="I7" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>RF connectors</t>
+        </is>
       </c>
     </row>
     <row r="8" spans="1:18" ht="13.5">
@@ -338,28 +357,33 @@
         </is>
       </c>
       <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SFM-110-01-S-D-LC</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>"Aux": TigerEye SFM series 20 pin 1.27 mm TH Vertical connector</t>
+        </is>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>SFM-110-01-S-D-LC-ND</t>
+        </is>
+      </c>
+      <c r="I8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>SFM-110-01-S-D-LC</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>"Aux": TigerEye SFM series 20 pin 1.27 mm TH Vertical connector</t>
-        </is>
-      </c>
-      <c r="G8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>SFM-110-01-S-D-LC-ND</t>
-        </is>
-      </c>
-      <c r="I8" t="s">
-        <v>2</v>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Auxiliary (not placed!)</t>
+        </is>
       </c>
     </row>
     <row r="9" spans="1:18" ht="13.5">
@@ -372,31 +396,36 @@
         </is>
       </c>
       <c r="C9" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>SFM-120-01-S-D-LC</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>"Main": TigerEye SFM series 40 pin 1.27 mm TH Vertical connector</t>
+        </is>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>SAM11706-ND</t>
+        </is>
+      </c>
+      <c r="I9" t="s">
         <v>3</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>SFM-120-01-S-D-LC</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>"Main": TigerEye SFM series 40 pin 1.27 mm TH Vertical connector</t>
-        </is>
-      </c>
-      <c r="G9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>SAM11706-ND</t>
-        </is>
-      </c>
-      <c r="I9" t="s">
-        <v>2</v>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Main card connectors</t>
+        </is>
       </c>
     </row>
     <row r="10" spans="1:18" ht="13.5">
@@ -409,7 +438,7 @@
         </is>
       </c>
       <c r="C10" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -427,7 +456,7 @@
         </is>
       </c>
       <c r="G10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -435,11 +464,11 @@
         </is>
       </c>
       <c r="I10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>High wattage</t>
+          <t>High wattage just in case</t>
         </is>
       </c>
     </row>
@@ -453,7 +482,7 @@
         </is>
       </c>
       <c r="C11" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -471,7 +500,7 @@
         </is>
       </c>
       <c r="G11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -479,7 +508,7 @@
         </is>
       </c>
       <c r="I11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -497,75 +526,184 @@
         </is>
       </c>
       <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>TE</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>5-104196-5</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>20 Position Receptacle Connector  Through Hole, Right Angle</t>
+        </is>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>A115240-ND</t>
+        </is>
+      </c>
+      <c r="I12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>-Z End Cap connector</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="13.5">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>J3</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Harwin</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>M50-3501042</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>20 Position Connector Header Through Hole 0.050" (1.27mm)</t>
+        </is>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>952-1386-ND</t>
+        </is>
+      </c>
+      <c r="I13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Debug connector</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="13.5">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Revision versioing infro</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="13.5">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
         <v>0</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>TE</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>5-104196-5</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>20 Position Receptacle Connector  Through Hole, Right Angle</t>
-        </is>
-      </c>
-      <c r="G12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>A115240-ND</t>
-        </is>
-      </c>
-      <c r="I12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="13.5">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Revision versioing infro</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="13.5">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Rev</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="13.5">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>1.0r0</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Initial BOM for 1U.</t>
-        </is>
       </c>
     </row>
     <row r="18" spans="1:18" ht="13.5">
       <c r="A18" t="inlineStr">
         <is>
+          <t>1.0r0</t>
+        </is>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Initial BOM for 1U.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="13.5">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>1.1r0</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Added -Z end cap connector</t>
-        </is>
-      </c>
-    </row>
-    <row r="1048560" spans="1:18">
-      <c r="I1048560" s="0"/>
+      <c r="B19" s="4">
+        <v>44173</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Added -Z end cap connector, and debug connector.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="B36" s="4"/>
     </row>
     <row r="1048561" spans="1:18">
       <c r="I1048561" s="0"/>

</xml_diff>